<commit_message>
BUILD EXEC TUDO FUNCIONAL
</commit_message>
<xml_diff>
--- a/CHECKLIST-ALFA-1/Dados/registos_checklist.xlsx
+++ b/CHECKLIST-ALFA-1/Dados/registos_checklist.xlsx
@@ -483,7 +483,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -510,9 +510,10 @@
     <col width="8" customWidth="1" min="16" max="16"/>
     <col width="10" customWidth="1" min="17" max="17"/>
     <col width="12" customWidth="1" min="18" max="18"/>
-    <col width="8" customWidth="1" min="19" max="19"/>
-    <col width="14" customWidth="1" min="20" max="20"/>
-    <col width="30" customWidth="1" min="21" max="21"/>
+    <col width="10" customWidth="1" min="19" max="19"/>
+    <col width="8" customWidth="1" min="20" max="20"/>
+    <col width="14" customWidth="1" min="21" max="21"/>
+    <col width="30" customWidth="1" min="22" max="22"/>
   </cols>
   <sheetData>
     <row r="1" ht="25" customHeight="1">
@@ -608,15 +609,20 @@
       </c>
       <c r="S1" s="1" t="inlineStr">
         <is>
+          <t>Colunas</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
           <t>USB</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="U1" s="1" t="inlineStr">
         <is>
           <t>Portas de Vídeo</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>Notas</t>
         </is>
@@ -705,17 +711,18 @@
           <t>✓</t>
         </is>
       </c>
-      <c r="S2" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="S2" s="4" t="inlineStr"/>
       <c r="T2" s="3" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
-      <c r="U2" s="4" t="inlineStr">
+      <c r="U2" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="V2" s="4" t="inlineStr">
         <is>
           <t>testes</t>
         </is>
@@ -804,17 +811,18 @@
           <t>✓</t>
         </is>
       </c>
-      <c r="S3" s="6" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="S3" s="7" t="inlineStr"/>
       <c r="T3" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
-      <c r="U3" s="7" t="inlineStr">
+      <c r="U3" s="6" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="V3" s="7" t="inlineStr">
         <is>
           <t>Danos para teste</t>
         </is>
@@ -903,17 +911,18 @@
           <t>✓</t>
         </is>
       </c>
-      <c r="S4" s="3" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="S4" s="4" t="inlineStr"/>
       <c r="T4" s="3" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
-      <c r="U4" s="4" t="inlineStr">
+      <c r="U4" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="V4" s="4" t="inlineStr">
         <is>
           <t>teste</t>
         </is>
@@ -1006,19 +1015,128 @@
           <t>✓</t>
         </is>
       </c>
-      <c r="S5" s="6" t="inlineStr">
-        <is>
-          <t>✓</t>
-        </is>
-      </c>
+      <c r="S5" s="7" t="inlineStr"/>
       <c r="T5" s="6" t="inlineStr">
         <is>
           <t>✓</t>
         </is>
       </c>
-      <c r="U5" s="7" t="inlineStr">
+      <c r="U5" s="6" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="V5" s="7" t="inlineStr">
         <is>
           <t>teste</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="20" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>19/02/2026 21:53</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="inlineStr">
+        <is>
+          <t>Guilherme</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>ASUS System Product Name</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>221011108801049</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>AMD Ryzen 7 5800X3D 8-Core Processor</t>
+        </is>
+      </c>
+      <c r="G6" s="2" t="inlineStr">
+        <is>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="H6" s="2" t="inlineStr">
+        <is>
+          <t>DIMM</t>
+        </is>
+      </c>
+      <c r="I6" s="2" t="inlineStr"/>
+      <c r="J6" s="2" t="inlineStr">
+        <is>
+          <t>WD Blue SN570 1TB (932 GB) + Verbatim Vi550 S3 (477 GB)</t>
+        </is>
+      </c>
+      <c r="K6" s="2" t="inlineStr">
+        <is>
+          <t>NVIDIA GeForce RTX 3070</t>
+        </is>
+      </c>
+      <c r="L6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="M6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="N6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="O6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="P6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="Q6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="R6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="S6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="T6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="U6" s="3" t="inlineStr">
+        <is>
+          <t>✓</t>
+        </is>
+      </c>
+      <c r="V6" s="4" t="inlineStr">
+        <is>
+          <t>Sem observações</t>
         </is>
       </c>
     </row>

</xml_diff>